<commit_message>
fix the bug of calculating the bat_e_termin
</commit_message>
<xml_diff>
--- a/output/experiments/thesis_topic3/6h-bat-6weeks-disturbance-type-debug2.xlsx
+++ b/output/experiments/thesis_topic3/6h-bat-6weeks-disturbance-type-debug2.xlsx
@@ -16,6 +16,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="102">
   <si>
+    <t>id</t>
+  </si>
+  <si>
     <t>status</t>
   </si>
   <si>
@@ -179,9 +182,6 @@
   </si>
   <si>
     <t>load_pv_error_max_pos</t>
-  </si>
-  <si>
-    <t>id</t>
   </si>
   <si>
     <t>R</t>
@@ -677,16 +677,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BD31"/>
+  <dimension ref="A1:BE31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:56">
-      <c r="A1" s="1" t="s">
-        <v>55</v>
-      </c>
+    <row r="1" spans="1:57">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -852,3292 +849,3385 @@
       <c r="BD1" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="BE1" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="2" spans="1:56">
+    <row r="2" spans="1:57">
       <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>56</v>
       </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
       <c r="D2" t="s">
         <v>58</v>
       </c>
       <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
         <v>59</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>60</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>61</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>438</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>62</v>
       </c>
-      <c r="J2" t="s">
-        <v>63</v>
-      </c>
       <c r="K2" t="s">
         <v>63</v>
       </c>
       <c r="L2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" t="s">
         <v>64</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>65</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>3</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>2.5</v>
       </c>
-      <c r="P2">
-        <v>0.6</v>
-      </c>
       <c r="Q2">
         <v>0.6</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2">
+        <v>0.6</v>
+      </c>
+      <c r="S2" t="s">
         <v>66</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>67</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>0.2</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>70</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:56">
+    <row r="3" spans="1:57">
       <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
       <c r="D3" t="s">
         <v>58</v>
       </c>
       <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
         <v>59</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>60</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>61</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>438</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>62</v>
       </c>
-      <c r="J3" t="s">
-        <v>63</v>
-      </c>
       <c r="K3" t="s">
         <v>63</v>
       </c>
       <c r="L3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" t="s">
         <v>64</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>65</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>3</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>2.5</v>
       </c>
-      <c r="P3">
-        <v>0.6</v>
-      </c>
       <c r="Q3">
         <v>0.6</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3">
+        <v>0.6</v>
+      </c>
+      <c r="S3" t="s">
         <v>66</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>67</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>0.25</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>70</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:56">
+    <row r="4" spans="1:57">
       <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
       <c r="D4" t="s">
         <v>58</v>
       </c>
       <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
         <v>59</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>60</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>61</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>438</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>62</v>
       </c>
-      <c r="J4" t="s">
-        <v>63</v>
-      </c>
       <c r="K4" t="s">
         <v>63</v>
       </c>
       <c r="L4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" t="s">
         <v>64</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>65</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>3</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>2.5</v>
       </c>
-      <c r="P4">
-        <v>0.6</v>
-      </c>
       <c r="Q4">
         <v>0.6</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4">
+        <v>0.6</v>
+      </c>
+      <c r="S4" t="s">
         <v>66</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>67</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>0.3</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>70</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>432.5791151665703</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>6.989583333333333</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>870.0920569000001</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>74</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>432.5791151665703</v>
       </c>
-      <c r="AA4">
-        <v>414.5791151665703</v>
-      </c>
       <c r="AB4">
-        <v>18</v>
+        <v>419.3719151535422</v>
       </c>
       <c r="AC4">
         <v>18</v>
       </c>
       <c r="AD4">
+        <v>18</v>
+      </c>
+      <c r="AE4">
         <v>438</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>5.431951581335221</v>
       </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
       <c r="AG4">
         <v>0</v>
       </c>
       <c r="AH4">
-        <v>0.1677226560523087</v>
+        <v>0</v>
       </c>
       <c r="AI4">
         <v>0.1677226560523087</v>
       </c>
       <c r="AJ4">
+        <v>0.1677226560523087</v>
+      </c>
+      <c r="AK4">
         <v>0.1607435678275361</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <v>151.0850750743209</v>
       </c>
-      <c r="AM4">
+      <c r="AN4">
         <v>269.0870292944375</v>
       </c>
-      <c r="AO4">
+      <c r="AP4">
         <v>73.10879284649776</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <v>1935.216071535023</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>643.9173940813289</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>2579.133465616352</v>
       </c>
-      <c r="AS4">
+      <c r="AT4">
         <v>782.8247039997368</v>
       </c>
-      <c r="AT4">
+      <c r="AU4">
         <v>1886.018877142718</v>
       </c>
-      <c r="AU4">
+      <c r="AV4">
         <v>65.11898182603289</v>
       </c>
-      <c r="AV4">
+      <c r="AW4">
         <v>278.3389494694874</v>
       </c>
-      <c r="AW4">
+      <c r="AX4">
         <v>9.251920175049957</v>
       </c>
-      <c r="AX4">
+      <c r="AY4">
         <v>251.8084584572014</v>
       </c>
-      <c r="AY4">
+      <c r="AZ4">
         <v>32.98379112909279</v>
       </c>
-      <c r="AZ4">
+      <c r="BA4">
         <v>5.592989202188023</v>
       </c>
-      <c r="BA4">
+      <c r="BB4">
         <v>-96.15314729619588</v>
       </c>
-      <c r="BB4">
+      <c r="BC4">
         <v>127.436725496304</v>
       </c>
-      <c r="BC4">
-        <v>0</v>
-      </c>
       <c r="BD4">
         <v>0</v>
       </c>
+      <c r="BE4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:56">
+    <row r="5" spans="1:57">
       <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
       <c r="D5" t="s">
         <v>58</v>
       </c>
       <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" t="s">
         <v>59</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>60</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>61</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>438</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>62</v>
       </c>
-      <c r="J5" t="s">
-        <v>63</v>
-      </c>
       <c r="K5" t="s">
         <v>63</v>
       </c>
       <c r="L5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M5" t="s">
         <v>64</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>65</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>3</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>2.5</v>
       </c>
-      <c r="P5">
-        <v>0.6</v>
-      </c>
       <c r="Q5">
         <v>0.6</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5">
+        <v>0.6</v>
+      </c>
+      <c r="S5" t="s">
         <v>66</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>67</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>0.35</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>70</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>443.5077402461957</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>6.989583333333333</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>958.1754901</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>75</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>443.5077402461957</v>
       </c>
-      <c r="AA5">
-        <v>425.5077402461957</v>
-      </c>
       <c r="AB5">
-        <v>18</v>
+        <v>426.6796396453024</v>
       </c>
       <c r="AC5">
         <v>18</v>
       </c>
       <c r="AD5">
+        <v>18</v>
+      </c>
+      <c r="AE5">
         <v>438</v>
       </c>
-      <c r="AE5">
+      <c r="AF5">
         <v>5.431951581335221</v>
       </c>
-      <c r="AF5">
-        <v>0</v>
-      </c>
       <c r="AG5">
         <v>0</v>
       </c>
       <c r="AH5">
-        <v>0.171959980419318</v>
+        <v>0</v>
       </c>
       <c r="AI5">
         <v>0.171959980419318</v>
       </c>
       <c r="AJ5">
+        <v>0.171959980419318</v>
+      </c>
+      <c r="AK5">
         <v>0.1649808921945455</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <v>157.3378861274064</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>269.5374097653991</v>
       </c>
-      <c r="AO5">
+      <c r="AP5">
         <v>73.10879284649776</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <v>1935.216071535023</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>643.9173940813289</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>2579.133465616352</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>782.8247039997368</v>
       </c>
-      <c r="AT5">
+      <c r="AU5">
         <v>1897.665997291987</v>
       </c>
-      <c r="AU5">
+      <c r="AV5">
         <v>80.86283449102427</v>
       </c>
-      <c r="AV5">
+      <c r="AW5">
         <v>281.0178942595936</v>
       </c>
-      <c r="AW5">
+      <c r="AX5">
         <v>11.48048449419452</v>
       </c>
-      <c r="AX5">
+      <c r="AY5">
         <v>262.2298102123441</v>
       </c>
-      <c r="AY5">
+      <c r="AZ5">
         <v>8.06494848721356</v>
       </c>
-      <c r="AZ5">
+      <c r="BA5">
         <v>1.367555646609769</v>
       </c>
-      <c r="BA5">
+      <c r="BB5">
         <v>-131.605720536049</v>
       </c>
-      <c r="BB5">
+      <c r="BC5">
         <v>114.6461176408674</v>
       </c>
-      <c r="BC5">
-        <v>0</v>
-      </c>
       <c r="BD5">
         <v>0</v>
       </c>
+      <c r="BE5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:56">
+    <row r="6" spans="1:57">
       <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
       <c r="D6" t="s">
         <v>58</v>
       </c>
       <c r="E6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" t="s">
         <v>59</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>60</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>61</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>438</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>62</v>
       </c>
-      <c r="J6" t="s">
-        <v>63</v>
-      </c>
       <c r="K6" t="s">
         <v>63</v>
       </c>
       <c r="L6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M6" t="s">
         <v>64</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>65</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>3</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>2.5</v>
       </c>
-      <c r="P6">
-        <v>0.6</v>
-      </c>
       <c r="Q6">
         <v>0.6</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6">
+        <v>0.6</v>
+      </c>
+      <c r="S6" t="s">
         <v>66</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>67</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>0.4</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>70</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>466.6636239576612</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>6.989583333333333</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>959.7466932999999</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>76</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <v>466.6636239576612</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <v>448.6636239576612</v>
-      </c>
-      <c r="AB6">
-        <v>18</v>
       </c>
       <c r="AC6">
         <v>18</v>
       </c>
       <c r="AD6">
+        <v>18</v>
+      </c>
+      <c r="AE6">
         <v>438</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <v>5.431951581335221</v>
       </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
       <c r="AG6">
         <v>0</v>
       </c>
       <c r="AH6">
-        <v>0.1809381446051454</v>
+        <v>0</v>
       </c>
       <c r="AI6">
         <v>0.1809381446051454</v>
       </c>
       <c r="AJ6">
+        <v>0.1809381446051454</v>
+      </c>
+      <c r="AK6">
         <v>0.1739590563803728</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>177.9254780477949</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>270.7381459098663</v>
       </c>
-      <c r="AO6">
+      <c r="AP6">
         <v>73.10879284649776</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <v>1935.216071535023</v>
       </c>
-      <c r="AQ6">
+      <c r="AR6">
         <v>643.9173940813292</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <v>2579.133465616352</v>
       </c>
-      <c r="AS6">
+      <c r="AT6">
         <v>782.8247039997368</v>
       </c>
-      <c r="AT6">
+      <c r="AU6">
         <v>1898.934977793655</v>
       </c>
-      <c r="AU6">
+      <c r="AV6">
         <v>83.18510080592901</v>
       </c>
-      <c r="AV6">
+      <c r="AW6">
         <v>281.9057100107415</v>
       </c>
-      <c r="AW6">
+      <c r="AX6">
         <v>11.16756410087517</v>
       </c>
-      <c r="AX6">
+      <c r="AY6">
         <v>296.5424634129916</v>
       </c>
-      <c r="AY6">
-        <v>0</v>
-      </c>
       <c r="AZ6">
         <v>0</v>
       </c>
       <c r="BA6">
+        <v>0</v>
+      </c>
+      <c r="BB6">
         <v>-149.2947136856207</v>
       </c>
-      <c r="BB6">
+      <c r="BC6">
         <v>152.5156767593642</v>
       </c>
-      <c r="BC6">
-        <v>0</v>
-      </c>
       <c r="BD6">
         <v>0</v>
       </c>
+      <c r="BE6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:56">
+    <row r="7" spans="1:57">
       <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
-        <v>58</v>
-      </c>
       <c r="D7" t="s">
         <v>58</v>
       </c>
       <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
         <v>59</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>60</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>61</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>438</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>62</v>
       </c>
-      <c r="J7" t="s">
-        <v>63</v>
-      </c>
       <c r="K7" t="s">
         <v>63</v>
       </c>
       <c r="L7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" t="s">
         <v>64</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>65</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>3</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>2.5</v>
       </c>
-      <c r="P7">
-        <v>0.6</v>
-      </c>
       <c r="Q7">
         <v>0.6</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7">
+        <v>0.6</v>
+      </c>
+      <c r="S7" t="s">
         <v>66</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>67</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>0.2</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>71</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:56">
+    <row r="8" spans="1:57">
       <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>56</v>
       </c>
-      <c r="C8" t="s">
-        <v>58</v>
-      </c>
       <c r="D8" t="s">
         <v>58</v>
       </c>
       <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
         <v>59</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>60</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>61</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>438</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>62</v>
       </c>
-      <c r="J8" t="s">
-        <v>63</v>
-      </c>
       <c r="K8" t="s">
         <v>63</v>
       </c>
       <c r="L8" t="s">
+        <v>63</v>
+      </c>
+      <c r="M8" t="s">
         <v>64</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>65</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>3</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>2.5</v>
       </c>
-      <c r="P8">
-        <v>0.6</v>
-      </c>
       <c r="Q8">
         <v>0.6</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8">
+        <v>0.6</v>
+      </c>
+      <c r="S8" t="s">
         <v>66</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>67</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>0.25</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>71</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:56">
+    <row r="9" spans="1:57">
       <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>56</v>
       </c>
-      <c r="C9" t="s">
-        <v>58</v>
-      </c>
       <c r="D9" t="s">
         <v>58</v>
       </c>
       <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
         <v>59</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>60</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>61</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>438</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>62</v>
       </c>
-      <c r="J9" t="s">
-        <v>63</v>
-      </c>
       <c r="K9" t="s">
         <v>63</v>
       </c>
       <c r="L9" t="s">
+        <v>63</v>
+      </c>
+      <c r="M9" t="s">
         <v>64</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>65</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>3</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>2.5</v>
       </c>
-      <c r="P9">
-        <v>0.6</v>
-      </c>
       <c r="Q9">
         <v>0.6</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9">
+        <v>0.6</v>
+      </c>
+      <c r="S9" t="s">
         <v>66</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>67</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>0.3</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>71</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:56">
+    <row r="10" spans="1:57">
       <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>56</v>
       </c>
-      <c r="C10" t="s">
-        <v>58</v>
-      </c>
       <c r="D10" t="s">
         <v>58</v>
       </c>
       <c r="E10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" t="s">
         <v>59</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>60</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>61</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>438</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>62</v>
       </c>
-      <c r="J10" t="s">
-        <v>63</v>
-      </c>
       <c r="K10" t="s">
         <v>63</v>
       </c>
       <c r="L10" t="s">
+        <v>63</v>
+      </c>
+      <c r="M10" t="s">
         <v>64</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>65</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>3</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>2.5</v>
       </c>
-      <c r="P10">
-        <v>0.6</v>
-      </c>
       <c r="Q10">
         <v>0.6</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10">
+        <v>0.6</v>
+      </c>
+      <c r="S10" t="s">
         <v>66</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>67</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>0.35</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>71</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:56">
+    <row r="11" spans="1:57">
       <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>56</v>
       </c>
-      <c r="C11" t="s">
-        <v>58</v>
-      </c>
       <c r="D11" t="s">
         <v>58</v>
       </c>
       <c r="E11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
         <v>59</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>60</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>61</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>438</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>62</v>
       </c>
-      <c r="J11" t="s">
-        <v>63</v>
-      </c>
       <c r="K11" t="s">
         <v>63</v>
       </c>
       <c r="L11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" t="s">
         <v>64</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>65</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>3</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>2.5</v>
       </c>
-      <c r="P11">
-        <v>0.6</v>
-      </c>
       <c r="Q11">
         <v>0.6</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11">
+        <v>0.6</v>
+      </c>
+      <c r="S11" t="s">
         <v>66</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>67</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>0.4</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>71</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Z11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:56">
+    <row r="12" spans="1:57">
       <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>57</v>
       </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
       <c r="D12" t="s">
         <v>58</v>
       </c>
       <c r="E12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" t="s">
         <v>59</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>60</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>61</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>438</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>62</v>
       </c>
-      <c r="J12" t="s">
-        <v>63</v>
-      </c>
       <c r="K12" t="s">
         <v>63</v>
       </c>
       <c r="L12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" t="s">
         <v>64</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>65</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>3</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>2.5</v>
       </c>
-      <c r="P12">
-        <v>0.6</v>
-      </c>
       <c r="Q12">
         <v>0.6</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12">
+        <v>0.6</v>
+      </c>
+      <c r="S12" t="s">
         <v>66</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>68</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>0.2</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>70</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>385.2683977279413</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>6.989583333333333</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <v>1488.3450243</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Z12" t="s">
         <v>82</v>
       </c>
-      <c r="Z12">
+      <c r="AA12">
         <v>385.2683977279413</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <v>367.2683977279413</v>
-      </c>
-      <c r="AB12">
-        <v>18</v>
       </c>
       <c r="AC12">
         <v>18</v>
       </c>
       <c r="AD12">
+        <v>18</v>
+      </c>
+      <c r="AE12">
         <v>438</v>
       </c>
-      <c r="AE12">
+      <c r="AF12">
         <v>5.431951581335221</v>
       </c>
-      <c r="AF12">
-        <v>0</v>
-      </c>
       <c r="AG12">
         <v>0</v>
       </c>
       <c r="AH12">
-        <v>0.1493790076644488</v>
+        <v>0</v>
       </c>
       <c r="AI12">
         <v>0.1493790076644488</v>
       </c>
       <c r="AJ12">
+        <v>0.1493790076644488</v>
+      </c>
+      <c r="AK12">
         <v>0.1423999194396762</v>
       </c>
-      <c r="AL12">
+      <c r="AM12">
         <v>101.6367679192026</v>
       </c>
-      <c r="AM12">
+      <c r="AN12">
         <v>265.6316298087388</v>
       </c>
-      <c r="AO12">
+      <c r="AP12">
         <v>73.10879284649776</v>
       </c>
-      <c r="AP12">
+      <c r="AQ12">
         <v>1935.216071535023</v>
       </c>
-      <c r="AQ12">
+      <c r="AR12">
         <v>643.9173940813286</v>
       </c>
-      <c r="AR12">
+      <c r="AS12">
         <v>2579.133465616351</v>
       </c>
-      <c r="AS12">
+      <c r="AT12">
         <v>782.8247039997368</v>
       </c>
-      <c r="AT12">
+      <c r="AU12">
         <v>1895.910254728095</v>
       </c>
-      <c r="AU12">
+      <c r="AV12">
         <v>79.14908907571791</v>
       </c>
-      <c r="AV12">
+      <c r="AW12">
         <v>277.1445488304431</v>
       </c>
-      <c r="AW12">
+      <c r="AX12">
         <v>11.51291902170435</v>
       </c>
-      <c r="AX12">
+      <c r="AY12">
         <v>169.394613198671</v>
       </c>
-      <c r="AY12">
-        <v>0</v>
-      </c>
       <c r="AZ12">
         <v>0</v>
       </c>
       <c r="BA12">
+        <v>0</v>
+      </c>
+      <c r="BB12">
         <v>-42.02111930425859</v>
       </c>
-      <c r="BB12">
-        <v>0</v>
-      </c>
       <c r="BC12">
         <v>0</v>
       </c>
       <c r="BD12">
         <v>0</v>
       </c>
+      <c r="BE12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:56">
+    <row r="13" spans="1:57">
       <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>57</v>
       </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
       <c r="D13" t="s">
         <v>58</v>
       </c>
       <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" t="s">
         <v>59</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>60</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>61</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>438</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>62</v>
       </c>
-      <c r="J13" t="s">
-        <v>63</v>
-      </c>
       <c r="K13" t="s">
         <v>63</v>
       </c>
       <c r="L13" t="s">
+        <v>63</v>
+      </c>
+      <c r="M13" t="s">
         <v>64</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>65</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>3</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>2.5</v>
       </c>
-      <c r="P13">
-        <v>0.6</v>
-      </c>
       <c r="Q13">
         <v>0.6</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13">
+        <v>0.6</v>
+      </c>
+      <c r="S13" t="s">
         <v>66</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>68</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>0.25</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>70</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>389.8508782814731</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>6.989583333333333</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <v>1483.9088014</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Z13" t="s">
         <v>83</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>389.8508782814731</v>
       </c>
-      <c r="AA13">
-        <v>371.8508782814731</v>
-      </c>
       <c r="AB13">
-        <v>18</v>
+        <v>371.9145052177852</v>
       </c>
       <c r="AC13">
         <v>18</v>
       </c>
       <c r="AD13">
+        <v>18</v>
+      </c>
+      <c r="AE13">
         <v>438</v>
       </c>
-      <c r="AE13">
+      <c r="AF13">
         <v>5.431951581335221</v>
       </c>
-      <c r="AF13">
-        <v>0</v>
-      </c>
       <c r="AG13">
         <v>0</v>
       </c>
       <c r="AH13">
-        <v>0.1511557596684156</v>
+        <v>0</v>
       </c>
       <c r="AI13">
         <v>0.1511557596684156</v>
       </c>
       <c r="AJ13">
+        <v>0.1511557596684156</v>
+      </c>
+      <c r="AK13">
         <v>0.144176671443643</v>
       </c>
-      <c r="AL13">
+      <c r="AM13">
         <v>104.8640338864866</v>
       </c>
-      <c r="AM13">
+      <c r="AN13">
         <v>267.0610942632741</v>
       </c>
-      <c r="AO13">
+      <c r="AP13">
         <v>73.10879284649776</v>
       </c>
-      <c r="AP13">
+      <c r="AQ13">
         <v>1935.216071535023</v>
       </c>
-      <c r="AQ13">
+      <c r="AR13">
         <v>643.9173940813289</v>
       </c>
-      <c r="AR13">
+      <c r="AS13">
         <v>2579.133465616352</v>
       </c>
-      <c r="AS13">
+      <c r="AT13">
         <v>782.8247039997368</v>
       </c>
-      <c r="AT13">
+      <c r="AU13">
         <v>1922.169658404883</v>
       </c>
-      <c r="AU13">
+      <c r="AV13">
         <v>105.5464951630463</v>
       </c>
-      <c r="AV13">
+      <c r="AW13">
         <v>282.4071798654846</v>
       </c>
-      <c r="AW13">
+      <c r="AX13">
         <v>15.3460856022105</v>
       </c>
-      <c r="AX13">
+      <c r="AY13">
         <v>174.7733898108111</v>
       </c>
-      <c r="AY13">
+      <c r="AZ13">
         <v>0.4378771455531236</v>
       </c>
-      <c r="AZ13">
+      <c r="BA13">
         <v>0.07424986828768139</v>
       </c>
-      <c r="BA13">
+      <c r="BB13">
         <v>-53.16114386753645</v>
       </c>
-      <c r="BB13">
-        <v>0</v>
-      </c>
       <c r="BC13">
         <v>0</v>
       </c>
       <c r="BD13">
         <v>0</v>
       </c>
+      <c r="BE13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:56">
+    <row r="14" spans="1:57">
       <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>57</v>
       </c>
-      <c r="C14" t="s">
-        <v>58</v>
-      </c>
       <c r="D14" t="s">
         <v>58</v>
       </c>
       <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
         <v>59</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>60</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>61</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>438</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>62</v>
       </c>
-      <c r="J14" t="s">
-        <v>63</v>
-      </c>
       <c r="K14" t="s">
         <v>63</v>
       </c>
       <c r="L14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M14" t="s">
         <v>64</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>65</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>3</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>2.5</v>
       </c>
-      <c r="P14">
-        <v>0.6</v>
-      </c>
       <c r="Q14">
         <v>0.6</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R14">
+        <v>0.6</v>
+      </c>
+      <c r="S14" t="s">
         <v>66</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>68</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>0.3</v>
       </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
         <v>70</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>389.4327981026314</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>6.989583333333333</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <v>1017.6225209</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="Z14" t="s">
         <v>84</v>
       </c>
-      <c r="Z14">
+      <c r="AA14">
         <v>389.4327981026314</v>
       </c>
-      <c r="AA14">
-        <v>371.4327981026314</v>
-      </c>
       <c r="AB14">
-        <v>18</v>
+        <v>373.6245703719802</v>
       </c>
       <c r="AC14">
         <v>18</v>
       </c>
       <c r="AD14">
+        <v>18</v>
+      </c>
+      <c r="AE14">
         <v>438</v>
       </c>
-      <c r="AE14">
+      <c r="AF14">
         <v>5.431951581335221</v>
       </c>
-      <c r="AF14">
-        <v>0</v>
-      </c>
       <c r="AG14">
         <v>0</v>
       </c>
       <c r="AH14">
-        <v>0.1509936586432398</v>
+        <v>0</v>
       </c>
       <c r="AI14">
         <v>0.1509936586432398</v>
       </c>
       <c r="AJ14">
+        <v>0.1509936586432398</v>
+      </c>
+      <c r="AK14">
         <v>0.1440145704184672</v>
       </c>
-      <c r="AL14">
+      <c r="AM14">
         <v>106.8893169788627</v>
       </c>
-      <c r="AM14">
+      <c r="AN14">
         <v>267.1011840676522</v>
       </c>
-      <c r="AO14">
+      <c r="AP14">
         <v>73.10879284649776</v>
       </c>
-      <c r="AP14">
+      <c r="AQ14">
         <v>1935.216071535023</v>
       </c>
-      <c r="AQ14">
+      <c r="AR14">
         <v>643.9173940813284</v>
       </c>
-      <c r="AR14">
+      <c r="AS14">
         <v>2579.133465616351</v>
       </c>
-      <c r="AS14">
+      <c r="AT14">
         <v>782.8247039997368</v>
       </c>
-      <c r="AT14">
+      <c r="AU14">
         <v>1932.616265971956</v>
       </c>
-      <c r="AU14">
+      <c r="AV14">
         <v>113.4870174319841</v>
       </c>
-      <c r="AV14">
+      <c r="AW14">
         <v>283.5872426109929</v>
       </c>
-      <c r="AW14">
+      <c r="AX14">
         <v>16.48605854334075</v>
       </c>
-      <c r="AX14">
+      <c r="AY14">
         <v>178.1488616314379</v>
       </c>
-      <c r="AY14">
+      <c r="AZ14">
         <v>15.08365859857521</v>
       </c>
-      <c r="AZ14">
+      <c r="BA14">
         <v>2.557702943883578</v>
       </c>
-      <c r="BA14">
+      <c r="BB14">
         <v>-59.849175534824</v>
       </c>
-      <c r="BB14">
-        <v>0</v>
-      </c>
       <c r="BC14">
         <v>0</v>
       </c>
       <c r="BD14">
         <v>0</v>
       </c>
+      <c r="BE14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:56">
+    <row r="15" spans="1:57">
       <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>57</v>
       </c>
-      <c r="C15" t="s">
-        <v>58</v>
-      </c>
       <c r="D15" t="s">
         <v>58</v>
       </c>
       <c r="E15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" t="s">
         <v>59</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>60</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>61</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>438</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>62</v>
       </c>
-      <c r="J15" t="s">
-        <v>63</v>
-      </c>
       <c r="K15" t="s">
         <v>63</v>
       </c>
       <c r="L15" t="s">
+        <v>63</v>
+      </c>
+      <c r="M15" t="s">
         <v>64</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>65</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>3</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>2.5</v>
       </c>
-      <c r="P15">
-        <v>0.6</v>
-      </c>
       <c r="Q15">
         <v>0.6</v>
       </c>
-      <c r="R15" t="s">
+      <c r="R15">
+        <v>0.6</v>
+      </c>
+      <c r="S15" t="s">
         <v>66</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>68</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>0.35</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>70</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>394.2691401102155</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>6.989583333333333</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <v>852.3801024999998</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Z15" t="s">
         <v>85</v>
       </c>
-      <c r="Z15">
+      <c r="AA15">
         <v>394.2691401102155</v>
       </c>
-      <c r="AA15">
+      <c r="AB15">
         <v>376.2691401102155</v>
-      </c>
-      <c r="AB15">
-        <v>18</v>
       </c>
       <c r="AC15">
         <v>18</v>
       </c>
       <c r="AD15">
+        <v>18</v>
+      </c>
+      <c r="AE15">
         <v>438</v>
       </c>
-      <c r="AE15">
+      <c r="AF15">
         <v>5.431951581335221</v>
       </c>
-      <c r="AF15">
-        <v>0</v>
-      </c>
       <c r="AG15">
         <v>0</v>
       </c>
       <c r="AH15">
-        <v>0.1528688396185789</v>
+        <v>0</v>
       </c>
       <c r="AI15">
         <v>0.1528688396185789</v>
       </c>
       <c r="AJ15">
+        <v>0.1528688396185789</v>
+      </c>
+      <c r="AK15">
         <v>0.1458897513938062</v>
       </c>
-      <c r="AL15">
+      <c r="AM15">
         <v>108.1877485401987</v>
       </c>
-      <c r="AM15">
+      <c r="AN15">
         <v>268.0813915700169</v>
       </c>
-      <c r="AO15">
+      <c r="AP15">
         <v>73.10879284649776</v>
       </c>
-      <c r="AP15">
+      <c r="AQ15">
         <v>1935.216071535023</v>
       </c>
-      <c r="AQ15">
+      <c r="AR15">
         <v>643.917394081329</v>
       </c>
-      <c r="AR15">
+      <c r="AS15">
         <v>2579.133465616352</v>
       </c>
-      <c r="AS15">
+      <c r="AT15">
         <v>782.8247039997368</v>
       </c>
-      <c r="AT15">
+      <c r="AU15">
         <v>1945.021599310056</v>
       </c>
-      <c r="AU15">
+      <c r="AV15">
         <v>128.0498515539489</v>
       </c>
-      <c r="AV15">
+      <c r="AW15">
         <v>286.4660265829269</v>
       </c>
-      <c r="AW15">
+      <c r="AX15">
         <v>18.38463501291008</v>
       </c>
-      <c r="AX15">
+      <c r="AY15">
         <v>180.3129142336645</v>
       </c>
-      <c r="AY15">
+      <c r="AZ15">
         <v>3.552713678800501E-15</v>
       </c>
-      <c r="AZ15">
+      <c r="BA15">
         <v>6.024258753709678E-16</v>
       </c>
-      <c r="BA15">
+      <c r="BB15">
         <v>-69.66158898676062</v>
       </c>
-      <c r="BB15">
-        <v>0</v>
-      </c>
       <c r="BC15">
         <v>0</v>
       </c>
       <c r="BD15">
         <v>0</v>
       </c>
+      <c r="BE15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:56">
+    <row r="16" spans="1:57">
       <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>57</v>
       </c>
-      <c r="C16" t="s">
-        <v>58</v>
-      </c>
       <c r="D16" t="s">
         <v>58</v>
       </c>
       <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" t="s">
         <v>59</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>60</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>61</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>438</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>62</v>
       </c>
-      <c r="J16" t="s">
-        <v>63</v>
-      </c>
       <c r="K16" t="s">
         <v>63</v>
       </c>
       <c r="L16" t="s">
+        <v>63</v>
+      </c>
+      <c r="M16" t="s">
         <v>64</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>65</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>3</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>2.5</v>
       </c>
-      <c r="P16">
-        <v>0.6</v>
-      </c>
       <c r="Q16">
         <v>0.6</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R16">
+        <v>0.6</v>
+      </c>
+      <c r="S16" t="s">
         <v>66</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>68</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>0.4</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>70</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>405.1933501008097</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>6.989583333333333</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <v>1326.3782173</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="Z16" t="s">
         <v>86</v>
       </c>
-      <c r="Z16">
+      <c r="AA16">
         <v>405.1933501008097</v>
       </c>
-      <c r="AA16">
+      <c r="AB16">
         <v>387.1933501008097</v>
-      </c>
-      <c r="AB16">
-        <v>18</v>
       </c>
       <c r="AC16">
         <v>18</v>
       </c>
       <c r="AD16">
+        <v>18</v>
+      </c>
+      <c r="AE16">
         <v>438</v>
       </c>
-      <c r="AE16">
+      <c r="AF16">
         <v>5.431951581335221</v>
       </c>
-      <c r="AF16">
-        <v>0</v>
-      </c>
       <c r="AG16">
         <v>0</v>
       </c>
       <c r="AH16">
-        <v>0.1571044521358177</v>
+        <v>0</v>
       </c>
       <c r="AI16">
         <v>0.1571044521358177</v>
       </c>
       <c r="AJ16">
+        <v>0.1571044521358177</v>
+      </c>
+      <c r="AK16">
         <v>0.1501253639110451</v>
       </c>
-      <c r="AL16">
+      <c r="AM16">
         <v>118.5513723007971</v>
       </c>
-      <c r="AM16">
+      <c r="AN16">
         <v>268.6419778000125</v>
       </c>
-      <c r="AO16">
+      <c r="AP16">
         <v>73.10879284649776</v>
       </c>
-      <c r="AP16">
+      <c r="AQ16">
         <v>1935.216071535023</v>
       </c>
-      <c r="AQ16">
+      <c r="AR16">
         <v>643.9173940813283</v>
       </c>
-      <c r="AR16">
+      <c r="AS16">
         <v>2579.133465616351</v>
       </c>
-      <c r="AS16">
+      <c r="AT16">
         <v>782.8247039997368</v>
       </c>
-      <c r="AT16">
+      <c r="AU16">
         <v>1950.904513722482</v>
       </c>
-      <c r="AU16">
+      <c r="AV16">
         <v>134.7669985790074</v>
       </c>
-      <c r="AV16">
+      <c r="AW16">
         <v>288.223447358293</v>
       </c>
-      <c r="AW16">
+      <c r="AX16">
         <v>19.58146955828042</v>
       </c>
-      <c r="AX16">
+      <c r="AY16">
         <v>197.5856205013285</v>
       </c>
-      <c r="AY16">
-        <v>0</v>
-      </c>
       <c r="AZ16">
         <v>0</v>
       </c>
       <c r="BA16">
+        <v>0</v>
+      </c>
+      <c r="BB16">
         <v>-83.82402666740754</v>
       </c>
-      <c r="BB16">
-        <v>0</v>
-      </c>
       <c r="BC16">
         <v>0</v>
       </c>
       <c r="BD16">
         <v>0</v>
       </c>
+      <c r="BE16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:56">
+    <row r="17" spans="1:57">
       <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>56</v>
       </c>
-      <c r="C17" t="s">
-        <v>58</v>
-      </c>
       <c r="D17" t="s">
         <v>58</v>
       </c>
       <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" t="s">
         <v>59</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>60</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>61</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>438</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>62</v>
       </c>
-      <c r="J17" t="s">
-        <v>63</v>
-      </c>
       <c r="K17" t="s">
         <v>63</v>
       </c>
       <c r="L17" t="s">
+        <v>63</v>
+      </c>
+      <c r="M17" t="s">
         <v>64</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>65</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>3</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>2.5</v>
       </c>
-      <c r="P17">
-        <v>0.6</v>
-      </c>
       <c r="Q17">
         <v>0.6</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17">
+        <v>0.6</v>
+      </c>
+      <c r="S17" t="s">
         <v>66</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>68</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>0.2</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>71</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="Z17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:56">
+    <row r="18" spans="1:57">
       <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>56</v>
       </c>
-      <c r="C18" t="s">
-        <v>58</v>
-      </c>
       <c r="D18" t="s">
         <v>58</v>
       </c>
       <c r="E18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" t="s">
         <v>59</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>60</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>61</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>438</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>62</v>
       </c>
-      <c r="J18" t="s">
-        <v>63</v>
-      </c>
       <c r="K18" t="s">
         <v>63</v>
       </c>
       <c r="L18" t="s">
+        <v>63</v>
+      </c>
+      <c r="M18" t="s">
         <v>64</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>65</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>3</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>2.5</v>
       </c>
-      <c r="P18">
-        <v>0.6</v>
-      </c>
       <c r="Q18">
         <v>0.6</v>
       </c>
-      <c r="R18" t="s">
+      <c r="R18">
+        <v>0.6</v>
+      </c>
+      <c r="S18" t="s">
         <v>66</v>
       </c>
-      <c r="S18" t="s">
+      <c r="T18" t="s">
         <v>68</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>0.25</v>
       </c>
-      <c r="U18" t="s">
+      <c r="V18" t="s">
         <v>71</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Z18" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:56">
+    <row r="19" spans="1:57">
       <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>56</v>
       </c>
-      <c r="C19" t="s">
-        <v>58</v>
-      </c>
       <c r="D19" t="s">
         <v>58</v>
       </c>
       <c r="E19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" t="s">
         <v>59</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>60</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>61</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>438</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>62</v>
       </c>
-      <c r="J19" t="s">
-        <v>63</v>
-      </c>
       <c r="K19" t="s">
         <v>63</v>
       </c>
       <c r="L19" t="s">
+        <v>63</v>
+      </c>
+      <c r="M19" t="s">
         <v>64</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>65</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>3</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>2.5</v>
       </c>
-      <c r="P19">
-        <v>0.6</v>
-      </c>
       <c r="Q19">
         <v>0.6</v>
       </c>
-      <c r="R19" t="s">
+      <c r="R19">
+        <v>0.6</v>
+      </c>
+      <c r="S19" t="s">
         <v>66</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>68</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>0.3</v>
       </c>
-      <c r="U19" t="s">
+      <c r="V19" t="s">
         <v>71</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="Z19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:56">
+    <row r="20" spans="1:57">
       <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>56</v>
       </c>
-      <c r="C20" t="s">
-        <v>58</v>
-      </c>
       <c r="D20" t="s">
         <v>58</v>
       </c>
       <c r="E20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" t="s">
         <v>59</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>60</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>61</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>438</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>62</v>
       </c>
-      <c r="J20" t="s">
-        <v>63</v>
-      </c>
       <c r="K20" t="s">
         <v>63</v>
       </c>
       <c r="L20" t="s">
+        <v>63</v>
+      </c>
+      <c r="M20" t="s">
         <v>64</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>65</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>3</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>2.5</v>
       </c>
-      <c r="P20">
-        <v>0.6</v>
-      </c>
       <c r="Q20">
         <v>0.6</v>
       </c>
-      <c r="R20" t="s">
+      <c r="R20">
+        <v>0.6</v>
+      </c>
+      <c r="S20" t="s">
         <v>66</v>
       </c>
-      <c r="S20" t="s">
+      <c r="T20" t="s">
         <v>68</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>0.35</v>
       </c>
-      <c r="U20" t="s">
+      <c r="V20" t="s">
         <v>71</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Z20" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:56">
+    <row r="21" spans="1:57">
       <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>56</v>
       </c>
-      <c r="C21" t="s">
-        <v>58</v>
-      </c>
       <c r="D21" t="s">
         <v>58</v>
       </c>
       <c r="E21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" t="s">
         <v>59</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>60</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>61</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>438</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>62</v>
       </c>
-      <c r="J21" t="s">
-        <v>63</v>
-      </c>
       <c r="K21" t="s">
         <v>63</v>
       </c>
       <c r="L21" t="s">
+        <v>63</v>
+      </c>
+      <c r="M21" t="s">
         <v>64</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>65</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>3</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>2.5</v>
       </c>
-      <c r="P21">
-        <v>0.6</v>
-      </c>
       <c r="Q21">
         <v>0.6</v>
       </c>
-      <c r="R21" t="s">
+      <c r="R21">
+        <v>0.6</v>
+      </c>
+      <c r="S21" t="s">
         <v>66</v>
       </c>
-      <c r="S21" t="s">
+      <c r="T21" t="s">
         <v>68</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <v>0.4</v>
       </c>
-      <c r="U21" t="s">
+      <c r="V21" t="s">
         <v>71</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Z21" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:56">
+    <row r="22" spans="1:57">
       <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>57</v>
       </c>
-      <c r="C22" t="s">
-        <v>58</v>
-      </c>
       <c r="D22" t="s">
         <v>58</v>
       </c>
       <c r="E22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" t="s">
         <v>59</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>60</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>61</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>438</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>62</v>
       </c>
-      <c r="J22" t="s">
-        <v>63</v>
-      </c>
       <c r="K22" t="s">
         <v>63</v>
       </c>
       <c r="L22" t="s">
+        <v>63</v>
+      </c>
+      <c r="M22" t="s">
         <v>64</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>65</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>3</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>2.5</v>
       </c>
-      <c r="P22">
-        <v>0.6</v>
-      </c>
       <c r="Q22">
         <v>0.6</v>
       </c>
-      <c r="R22" t="s">
+      <c r="R22">
+        <v>0.6</v>
+      </c>
+      <c r="S22" t="s">
         <v>66</v>
       </c>
-      <c r="S22" t="s">
+      <c r="T22" t="s">
         <v>69</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <v>0.2</v>
       </c>
-      <c r="U22" t="s">
+      <c r="V22" t="s">
         <v>70</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>380.6953448449357</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>6.989583333333333</v>
       </c>
-      <c r="X22">
+      <c r="Y22">
         <v>1484.9599091</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Z22" t="s">
         <v>92</v>
       </c>
-      <c r="Z22">
+      <c r="AA22">
         <v>380.6953448449357</v>
       </c>
-      <c r="AA22">
-        <v>362.6953448449357</v>
-      </c>
       <c r="AB22">
-        <v>18</v>
+        <v>372.3852055901934</v>
       </c>
       <c r="AC22">
         <v>18</v>
       </c>
       <c r="AD22">
+        <v>18</v>
+      </c>
+      <c r="AE22">
         <v>438</v>
       </c>
-      <c r="AE22">
+      <c r="AF22">
         <v>5.431951581335221</v>
       </c>
-      <c r="AF22">
-        <v>0</v>
-      </c>
       <c r="AG22">
         <v>0</v>
       </c>
       <c r="AH22">
-        <v>0.1476059110240573</v>
+        <v>0</v>
       </c>
       <c r="AI22">
         <v>0.1476059110240573</v>
       </c>
       <c r="AJ22">
+        <v>0.1476059110240573</v>
+      </c>
+      <c r="AK22">
         <v>0.1406268227992847</v>
       </c>
-      <c r="AL22">
+      <c r="AM22">
         <v>105.0886988429092</v>
       </c>
-      <c r="AM22">
+      <c r="AN22">
         <v>268.914292193449</v>
       </c>
-      <c r="AO22">
+      <c r="AP22">
         <v>73.10879284649776</v>
       </c>
-      <c r="AP22">
+      <c r="AQ22">
         <v>1935.216071535023</v>
       </c>
-      <c r="AQ22">
+      <c r="AR22">
         <v>643.9173940813283</v>
       </c>
-      <c r="AR22">
+      <c r="AS22">
         <v>2579.133465616351</v>
       </c>
-      <c r="AS22">
+      <c r="AT22">
         <v>782.8247039997368</v>
       </c>
-      <c r="AT22">
+      <c r="AU22">
         <v>1833.36156384795</v>
       </c>
-      <c r="AU22">
+      <c r="AV22">
         <v>10.29370919044712</v>
       </c>
-      <c r="AV22">
+      <c r="AW22">
         <v>270.6779122406124</v>
       </c>
-      <c r="AW22">
+      <c r="AX22">
         <v>1.763620047163399</v>
       </c>
-      <c r="AX22">
+      <c r="AY22">
         <v>175.1478314048487</v>
       </c>
-      <c r="AY22">
+      <c r="AZ22">
         <v>66.68509926564022</v>
       </c>
-      <c r="AZ22">
+      <c r="BA22">
         <v>11.30764619142252</v>
       </c>
-      <c r="BA22">
-        <v>0</v>
-      </c>
       <c r="BB22">
+        <v>0</v>
+      </c>
+      <c r="BC22">
         <v>41.95572387488531</v>
       </c>
-      <c r="BC22">
-        <v>0</v>
-      </c>
       <c r="BD22">
         <v>0</v>
       </c>
+      <c r="BE22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:56">
+    <row r="23" spans="1:57">
       <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>57</v>
       </c>
-      <c r="C23" t="s">
-        <v>58</v>
-      </c>
       <c r="D23" t="s">
         <v>58</v>
       </c>
       <c r="E23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" t="s">
         <v>59</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>60</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>61</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>438</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>62</v>
       </c>
-      <c r="J23" t="s">
-        <v>63</v>
-      </c>
       <c r="K23" t="s">
         <v>63</v>
       </c>
       <c r="L23" t="s">
+        <v>63</v>
+      </c>
+      <c r="M23" t="s">
         <v>64</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>65</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>3</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>2.5</v>
       </c>
-      <c r="P23">
-        <v>0.6</v>
-      </c>
       <c r="Q23">
         <v>0.6</v>
       </c>
-      <c r="R23" t="s">
+      <c r="R23">
+        <v>0.6</v>
+      </c>
+      <c r="S23" t="s">
         <v>66</v>
       </c>
-      <c r="S23" t="s">
+      <c r="T23" t="s">
         <v>69</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>0.25</v>
       </c>
-      <c r="U23" t="s">
+      <c r="V23" t="s">
         <v>70</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>378.3274093089746</v>
       </c>
-      <c r="W23">
+      <c r="X23">
         <v>6.989583333333333</v>
       </c>
-      <c r="X23">
+      <c r="Y23">
         <v>963.628381</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="Z23" t="s">
         <v>93</v>
       </c>
-      <c r="Z23">
+      <c r="AA23">
         <v>378.3274093089746</v>
       </c>
-      <c r="AA23">
-        <v>360.3274093089746</v>
-      </c>
       <c r="AB23">
-        <v>18</v>
+        <v>373.9550991950703</v>
       </c>
       <c r="AC23">
         <v>18</v>
       </c>
       <c r="AD23">
+        <v>18</v>
+      </c>
+      <c r="AE23">
         <v>438</v>
       </c>
-      <c r="AE23">
+      <c r="AF23">
         <v>5.431951581335221</v>
       </c>
-      <c r="AF23">
-        <v>0</v>
-      </c>
       <c r="AG23">
         <v>0</v>
       </c>
       <c r="AH23">
-        <v>0.1466877981898325</v>
+        <v>0</v>
       </c>
       <c r="AI23">
         <v>0.1466877981898325</v>
       </c>
       <c r="AJ23">
+        <v>0.1466877981898325</v>
+      </c>
+      <c r="AK23">
         <v>0.1397087099650599</v>
       </c>
-      <c r="AL23">
+      <c r="AM23">
         <v>104.6734166075899</v>
       </c>
-      <c r="AM23">
+      <c r="AN23">
         <v>271.5569142902023</v>
       </c>
-      <c r="AO23">
+      <c r="AP23">
         <v>73.10879284649776</v>
       </c>
-      <c r="AP23">
+      <c r="AQ23">
         <v>1935.216071535023</v>
       </c>
-      <c r="AQ23">
+      <c r="AR23">
         <v>643.9173940813284</v>
       </c>
-      <c r="AR23">
+      <c r="AS23">
         <v>2579.133465616351</v>
       </c>
-      <c r="AS23">
+      <c r="AT23">
         <v>782.8247039997368</v>
       </c>
-      <c r="AT23">
+      <c r="AU23">
         <v>1837.053798918709</v>
       </c>
-      <c r="AU23">
+      <c r="AV23">
         <v>9.523941431870826</v>
       </c>
-      <c r="AV23">
+      <c r="AW23">
         <v>273.2369375587843</v>
       </c>
-      <c r="AW23">
+      <c r="AX23">
         <v>1.680023268582013</v>
       </c>
-      <c r="AX23">
+      <c r="AY23">
         <v>174.4556943459833</v>
       </c>
-      <c r="AY23">
+      <c r="AZ23">
         <v>93.78502712336717</v>
       </c>
-      <c r="AZ23">
+      <c r="BA23">
         <v>15.9029215888177</v>
       </c>
-      <c r="BA23">
-        <v>0</v>
-      </c>
       <c r="BB23">
+        <v>0</v>
+      </c>
+      <c r="BC23">
         <v>49.93058652838124</v>
       </c>
-      <c r="BC23">
-        <v>0</v>
-      </c>
       <c r="BD23">
         <v>0</v>
       </c>
+      <c r="BE23">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:56">
+    <row r="24" spans="1:57">
       <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>57</v>
       </c>
-      <c r="C24" t="s">
-        <v>58</v>
-      </c>
       <c r="D24" t="s">
         <v>58</v>
       </c>
       <c r="E24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" t="s">
         <v>59</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>60</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>61</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>438</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>62</v>
       </c>
-      <c r="J24" t="s">
-        <v>63</v>
-      </c>
       <c r="K24" t="s">
         <v>63</v>
       </c>
       <c r="L24" t="s">
+        <v>63</v>
+      </c>
+      <c r="M24" t="s">
         <v>64</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>65</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>3</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>2.5</v>
       </c>
-      <c r="P24">
-        <v>0.6</v>
-      </c>
       <c r="Q24">
         <v>0.6</v>
       </c>
-      <c r="R24" t="s">
+      <c r="R24">
+        <v>0.6</v>
+      </c>
+      <c r="S24" t="s">
         <v>66</v>
       </c>
-      <c r="S24" t="s">
+      <c r="T24" t="s">
         <v>69</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>0.3</v>
       </c>
-      <c r="U24" t="s">
+      <c r="V24" t="s">
         <v>70</v>
       </c>
-      <c r="V24">
+      <c r="W24">
         <v>383.0083227440621</v>
       </c>
-      <c r="W24">
+      <c r="X24">
         <v>6.989583333333333</v>
       </c>
-      <c r="X24">
+      <c r="Y24">
         <v>1358.3961551</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="Z24" t="s">
         <v>94</v>
       </c>
-      <c r="Z24">
+      <c r="AA24">
         <v>383.0083227440621</v>
       </c>
-      <c r="AA24">
-        <v>365.0083227440621</v>
-      </c>
       <c r="AB24">
-        <v>18</v>
+        <v>379.9760378046053</v>
       </c>
       <c r="AC24">
         <v>18</v>
       </c>
       <c r="AD24">
+        <v>18</v>
+      </c>
+      <c r="AE24">
         <v>438</v>
       </c>
-      <c r="AE24">
+      <c r="AF24">
         <v>5.431951581335221</v>
       </c>
-      <c r="AF24">
-        <v>0</v>
-      </c>
       <c r="AG24">
         <v>0</v>
       </c>
       <c r="AH24">
-        <v>0.1485027152918324</v>
+        <v>0</v>
       </c>
       <c r="AI24">
         <v>0.1485027152918324</v>
       </c>
       <c r="AJ24">
+        <v>0.1485027152918324</v>
+      </c>
+      <c r="AK24">
         <v>0.1415236270670598</v>
       </c>
-      <c r="AL24">
+      <c r="AM24">
         <v>111.0146518622374</v>
       </c>
-      <c r="AM24">
+      <c r="AN24">
         <v>271.4603435872586</v>
       </c>
-      <c r="AO24">
+      <c r="AP24">
         <v>73.10879284649776</v>
       </c>
-      <c r="AP24">
+      <c r="AQ24">
         <v>1935.216071535023</v>
       </c>
-      <c r="AQ24">
+      <c r="AR24">
         <v>643.9173940813288</v>
       </c>
-      <c r="AR24">
+      <c r="AS24">
         <v>2579.133465616352</v>
       </c>
-      <c r="AS24">
+      <c r="AT24">
         <v>782.8247039997368</v>
       </c>
-      <c r="AT24">
+      <c r="AU24">
         <v>1840.139904154731</v>
       </c>
-      <c r="AU24">
+      <c r="AV24">
         <v>10.76210919630649</v>
       </c>
-      <c r="AV24">
+      <c r="AW24">
         <v>273.2748318750584</v>
       </c>
-      <c r="AW24">
+      <c r="AX24">
         <v>1.814488287799726</v>
       </c>
-      <c r="AX24">
+      <c r="AY24">
         <v>185.0244197703957</v>
       </c>
-      <c r="AY24">
+      <c r="AZ24">
         <v>103.0070081327665</v>
       </c>
-      <c r="AZ24">
+      <c r="BA24">
         <v>17.46667270543387</v>
       </c>
-      <c r="BA24">
-        <v>0</v>
-      </c>
       <c r="BB24">
+        <v>0</v>
+      </c>
+      <c r="BC24">
         <v>61.3167674435276</v>
       </c>
-      <c r="BC24">
-        <v>0</v>
-      </c>
       <c r="BD24">
         <v>0</v>
       </c>
+      <c r="BE24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:56">
+    <row r="25" spans="1:57">
       <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>57</v>
       </c>
-      <c r="C25" t="s">
-        <v>58</v>
-      </c>
       <c r="D25" t="s">
         <v>58</v>
       </c>
       <c r="E25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" t="s">
         <v>59</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>60</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>61</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>438</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>62</v>
       </c>
-      <c r="J25" t="s">
-        <v>63</v>
-      </c>
       <c r="K25" t="s">
         <v>63</v>
       </c>
       <c r="L25" t="s">
+        <v>63</v>
+      </c>
+      <c r="M25" t="s">
         <v>64</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>65</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>3</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>2.5</v>
       </c>
-      <c r="P25">
-        <v>0.6</v>
-      </c>
       <c r="Q25">
         <v>0.6</v>
       </c>
-      <c r="R25" t="s">
+      <c r="R25">
+        <v>0.6</v>
+      </c>
+      <c r="S25" t="s">
         <v>66</v>
       </c>
-      <c r="S25" t="s">
+      <c r="T25" t="s">
         <v>69</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <v>0.35</v>
       </c>
-      <c r="U25" t="s">
+      <c r="V25" t="s">
         <v>70</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <v>390.6716652286481</v>
       </c>
-      <c r="W25">
+      <c r="X25">
         <v>6.989583333333333</v>
       </c>
-      <c r="X25">
+      <c r="Y25">
         <v>977.8800845000001</v>
       </c>
-      <c r="Y25" t="s">
+      <c r="Z25" t="s">
         <v>95</v>
       </c>
-      <c r="Z25">
+      <c r="AA25">
         <v>390.6716652286481</v>
       </c>
-      <c r="AA25">
-        <v>372.6716652286481</v>
-      </c>
       <c r="AB25">
-        <v>18</v>
+        <v>387.9741858086359</v>
       </c>
       <c r="AC25">
         <v>18</v>
       </c>
       <c r="AD25">
+        <v>18</v>
+      </c>
+      <c r="AE25">
         <v>438</v>
       </c>
-      <c r="AE25">
+      <c r="AF25">
         <v>5.431951581335221</v>
       </c>
-      <c r="AF25">
-        <v>0</v>
-      </c>
       <c r="AG25">
         <v>0</v>
       </c>
       <c r="AH25">
-        <v>0.151474001030531</v>
+        <v>0</v>
       </c>
       <c r="AI25">
         <v>0.151474001030531</v>
       </c>
       <c r="AJ25">
+        <v>0.151474001030531</v>
+      </c>
+      <c r="AK25">
         <v>0.1444949128057584</v>
       </c>
-      <c r="AL25">
+      <c r="AM25">
         <v>114.7383762563053</v>
       </c>
-      <c r="AM25">
+      <c r="AN25">
         <v>275.7906651622068</v>
       </c>
-      <c r="AO25">
+      <c r="AP25">
         <v>73.10879284649776</v>
       </c>
-      <c r="AP25">
+      <c r="AQ25">
         <v>1935.216071535023</v>
       </c>
-      <c r="AQ25">
+      <c r="AR25">
         <v>643.9173940813281</v>
       </c>
-      <c r="AR25">
+      <c r="AS25">
         <v>2579.133465616351</v>
       </c>
-      <c r="AS25">
+      <c r="AT25">
         <v>782.8247039997368</v>
       </c>
-      <c r="AT25">
+      <c r="AU25">
         <v>1837.658803098062</v>
       </c>
-      <c r="AU25">
+      <c r="AV25">
         <v>9.523941431870826</v>
       </c>
-      <c r="AV25">
+      <c r="AW25">
         <v>277.4706884307888</v>
       </c>
-      <c r="AW25">
+      <c r="AX25">
         <v>1.680023268582013</v>
       </c>
-      <c r="AX25">
+      <c r="AY25">
         <v>191.2306270938421</v>
       </c>
-      <c r="AY25">
+      <c r="AZ25">
         <v>105.3111216681206</v>
       </c>
-      <c r="AZ25">
+      <c r="BA25">
         <v>17.85737618986396</v>
       </c>
-      <c r="BA25">
-        <v>0</v>
-      </c>
       <c r="BB25">
+        <v>0</v>
+      </c>
+      <c r="BC25">
         <v>72.50136932865743</v>
       </c>
-      <c r="BC25">
-        <v>0</v>
-      </c>
       <c r="BD25">
         <v>0</v>
       </c>
+      <c r="BE25">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:56">
+    <row r="26" spans="1:57">
       <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>57</v>
       </c>
-      <c r="C26" t="s">
-        <v>58</v>
-      </c>
       <c r="D26" t="s">
         <v>58</v>
       </c>
       <c r="E26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" t="s">
         <v>59</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>60</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>61</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>438</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>62</v>
       </c>
-      <c r="J26" t="s">
-        <v>63</v>
-      </c>
       <c r="K26" t="s">
         <v>63</v>
       </c>
       <c r="L26" t="s">
+        <v>63</v>
+      </c>
+      <c r="M26" t="s">
         <v>64</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>65</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>3</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>2.5</v>
       </c>
-      <c r="P26">
-        <v>0.6</v>
-      </c>
       <c r="Q26">
         <v>0.6</v>
       </c>
-      <c r="R26" t="s">
+      <c r="R26">
+        <v>0.6</v>
+      </c>
+      <c r="S26" t="s">
         <v>66</v>
       </c>
-      <c r="S26" t="s">
+      <c r="T26" t="s">
         <v>69</v>
       </c>
-      <c r="T26">
+      <c r="U26">
         <v>0.4</v>
       </c>
-      <c r="U26" t="s">
+      <c r="V26" t="s">
         <v>70</v>
       </c>
-      <c r="V26">
+      <c r="W26">
         <v>395.8457637364535</v>
       </c>
-      <c r="W26">
+      <c r="X26">
         <v>6.989583333333333</v>
       </c>
-      <c r="X26">
+      <c r="Y26">
         <v>939.7914128000002</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="Z26" t="s">
         <v>96</v>
       </c>
-      <c r="Z26">
+      <c r="AA26">
         <v>395.8457637364535</v>
       </c>
-      <c r="AA26">
-        <v>377.8457637364535</v>
-      </c>
       <c r="AB26">
-        <v>18</v>
+        <v>392.2767594694238</v>
       </c>
       <c r="AC26">
         <v>18</v>
       </c>
       <c r="AD26">
+        <v>18</v>
+      </c>
+      <c r="AE26">
         <v>438</v>
       </c>
-      <c r="AE26">
+      <c r="AF26">
         <v>5.431951581335221</v>
       </c>
-      <c r="AF26">
-        <v>0</v>
-      </c>
       <c r="AG26">
         <v>0</v>
       </c>
       <c r="AH26">
-        <v>0.1534801393621776</v>
+        <v>0</v>
       </c>
       <c r="AI26">
         <v>0.1534801393621776</v>
       </c>
       <c r="AJ26">
+        <v>0.1534801393621776</v>
+      </c>
+      <c r="AK26">
         <v>0.146501051137405</v>
       </c>
-      <c r="AL26">
+      <c r="AM26">
         <v>116.6093299098344</v>
       </c>
-      <c r="AM26">
+      <c r="AN26">
         <v>278.0767784123984</v>
       </c>
-      <c r="AO26">
+      <c r="AP26">
         <v>73.10879284649776</v>
       </c>
-      <c r="AP26">
+      <c r="AQ26">
         <v>1935.216071535023</v>
       </c>
-      <c r="AQ26">
+      <c r="AR26">
         <v>643.9173940813278</v>
       </c>
-      <c r="AR26">
+      <c r="AS26">
         <v>2579.133465616351</v>
       </c>
-      <c r="AS26">
+      <c r="AT26">
         <v>782.8247039997368</v>
       </c>
-      <c r="AT26">
+      <c r="AU26">
         <v>1837.625078556434</v>
       </c>
-      <c r="AU26">
+      <c r="AV26">
         <v>9.428561402064567</v>
       </c>
-      <c r="AV26">
+      <c r="AW26">
         <v>279.7399766437226</v>
       </c>
-      <c r="AW26">
+      <c r="AX26">
         <v>1.66319823132419</v>
       </c>
-      <c r="AX26">
+      <c r="AY26">
         <v>194.3488831830574</v>
       </c>
-      <c r="AY26">
+      <c r="AZ26">
         <v>99.31333465510602</v>
       </c>
-      <c r="AZ26">
+      <c r="BA26">
         <v>16.84034458577931</v>
       </c>
-      <c r="BA26">
-        <v>0</v>
-      </c>
       <c r="BB26">
+        <v>0</v>
+      </c>
+      <c r="BC26">
         <v>79.75785680649146</v>
       </c>
-      <c r="BC26">
-        <v>0</v>
-      </c>
       <c r="BD26">
         <v>0</v>
       </c>
+      <c r="BE26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:56">
+    <row r="27" spans="1:57">
       <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>56</v>
       </c>
-      <c r="C27" t="s">
-        <v>58</v>
-      </c>
       <c r="D27" t="s">
         <v>58</v>
       </c>
       <c r="E27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" t="s">
         <v>59</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>60</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>61</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>438</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>62</v>
       </c>
-      <c r="J27" t="s">
-        <v>63</v>
-      </c>
       <c r="K27" t="s">
         <v>63</v>
       </c>
       <c r="L27" t="s">
+        <v>63</v>
+      </c>
+      <c r="M27" t="s">
         <v>64</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>65</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>3</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>2.5</v>
       </c>
-      <c r="P27">
-        <v>0.6</v>
-      </c>
       <c r="Q27">
         <v>0.6</v>
       </c>
-      <c r="R27" t="s">
+      <c r="R27">
+        <v>0.6</v>
+      </c>
+      <c r="S27" t="s">
         <v>66</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" t="s">
         <v>69</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <v>0.2</v>
       </c>
-      <c r="U27" t="s">
+      <c r="V27" t="s">
         <v>71</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="Z27" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:56">
+    <row r="28" spans="1:57">
       <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>56</v>
       </c>
-      <c r="C28" t="s">
-        <v>58</v>
-      </c>
       <c r="D28" t="s">
         <v>58</v>
       </c>
       <c r="E28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" t="s">
         <v>59</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>60</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>61</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>438</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>62</v>
       </c>
-      <c r="J28" t="s">
-        <v>63</v>
-      </c>
       <c r="K28" t="s">
         <v>63</v>
       </c>
       <c r="L28" t="s">
+        <v>63</v>
+      </c>
+      <c r="M28" t="s">
         <v>64</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>65</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>3</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>2.5</v>
       </c>
-      <c r="P28">
-        <v>0.6</v>
-      </c>
       <c r="Q28">
         <v>0.6</v>
       </c>
-      <c r="R28" t="s">
+      <c r="R28">
+        <v>0.6</v>
+      </c>
+      <c r="S28" t="s">
         <v>66</v>
       </c>
-      <c r="S28" t="s">
+      <c r="T28" t="s">
         <v>69</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <v>0.25</v>
       </c>
-      <c r="U28" t="s">
+      <c r="V28" t="s">
         <v>71</v>
       </c>
-      <c r="Y28" t="s">
+      <c r="Z28" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:56">
+    <row r="29" spans="1:57">
       <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>56</v>
       </c>
-      <c r="C29" t="s">
-        <v>58</v>
-      </c>
       <c r="D29" t="s">
         <v>58</v>
       </c>
       <c r="E29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" t="s">
         <v>59</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>60</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>61</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>438</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>62</v>
       </c>
-      <c r="J29" t="s">
-        <v>63</v>
-      </c>
       <c r="K29" t="s">
         <v>63</v>
       </c>
       <c r="L29" t="s">
+        <v>63</v>
+      </c>
+      <c r="M29" t="s">
         <v>64</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>65</v>
       </c>
-      <c r="N29">
+      <c r="O29">
         <v>3</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>2.5</v>
       </c>
-      <c r="P29">
-        <v>0.6</v>
-      </c>
       <c r="Q29">
         <v>0.6</v>
       </c>
-      <c r="R29" t="s">
+      <c r="R29">
+        <v>0.6</v>
+      </c>
+      <c r="S29" t="s">
         <v>66</v>
       </c>
-      <c r="S29" t="s">
+      <c r="T29" t="s">
         <v>69</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>0.3</v>
       </c>
-      <c r="U29" t="s">
+      <c r="V29" t="s">
         <v>71</v>
       </c>
-      <c r="Y29" t="s">
+      <c r="Z29" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:56">
+    <row r="30" spans="1:57">
       <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>56</v>
       </c>
-      <c r="C30" t="s">
-        <v>58</v>
-      </c>
       <c r="D30" t="s">
         <v>58</v>
       </c>
       <c r="E30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" t="s">
         <v>59</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>60</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>61</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>438</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>62</v>
       </c>
-      <c r="J30" t="s">
-        <v>63</v>
-      </c>
       <c r="K30" t="s">
         <v>63</v>
       </c>
       <c r="L30" t="s">
+        <v>63</v>
+      </c>
+      <c r="M30" t="s">
         <v>64</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>65</v>
       </c>
-      <c r="N30">
+      <c r="O30">
         <v>3</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>2.5</v>
       </c>
-      <c r="P30">
-        <v>0.6</v>
-      </c>
       <c r="Q30">
         <v>0.6</v>
       </c>
-      <c r="R30" t="s">
+      <c r="R30">
+        <v>0.6</v>
+      </c>
+      <c r="S30" t="s">
         <v>66</v>
       </c>
-      <c r="S30" t="s">
+      <c r="T30" t="s">
         <v>69</v>
       </c>
-      <c r="T30">
+      <c r="U30">
         <v>0.35</v>
       </c>
-      <c r="U30" t="s">
+      <c r="V30" t="s">
         <v>71</v>
       </c>
-      <c r="Y30" t="s">
+      <c r="Z30" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:56">
+    <row r="31" spans="1:57">
       <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>56</v>
       </c>
-      <c r="C31" t="s">
-        <v>58</v>
-      </c>
       <c r="D31" t="s">
         <v>58</v>
       </c>
       <c r="E31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" t="s">
         <v>59</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>60</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>61</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>438</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>62</v>
       </c>
-      <c r="J31" t="s">
-        <v>63</v>
-      </c>
       <c r="K31" t="s">
         <v>63</v>
       </c>
       <c r="L31" t="s">
+        <v>63</v>
+      </c>
+      <c r="M31" t="s">
         <v>64</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>65</v>
       </c>
-      <c r="N31">
+      <c r="O31">
         <v>3</v>
       </c>
-      <c r="O31">
+      <c r="P31">
         <v>2.5</v>
       </c>
-      <c r="P31">
-        <v>0.6</v>
-      </c>
       <c r="Q31">
         <v>0.6</v>
       </c>
-      <c r="R31" t="s">
+      <c r="R31">
+        <v>0.6</v>
+      </c>
+      <c r="S31" t="s">
         <v>66</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>69</v>
       </c>
-      <c r="T31">
+      <c r="U31">
         <v>0.4</v>
       </c>
-      <c r="U31" t="s">
+      <c r="V31" t="s">
         <v>71</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="Z31" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>